<commit_message>
Worked on tarea 1
1e is missing and 2c needs a little bit more work
</commit_message>
<xml_diff>
--- a/Tarea_1/1.c.xlsx
+++ b/Tarea_1/1.c.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danjo\Documents\GitHub\Tareas_IPD445_Circuitos_Digitales\Tarea_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97EF5B57-BE09-401F-A766-5B92423731DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7087D2-5FA4-4AEF-B4F5-ED6C6BF120F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6371CE3A-D3A7-4834-AECF-25EDF39F7B1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Vds</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Vgs</t>
+  </si>
+  <si>
+    <t>nMOS</t>
+  </si>
+  <si>
+    <t>pMOS</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-CL"/>
-              <a:t>Id en el punto Vds = Vgs - Vt</a:t>
+              <a:t>Id en el punto Vds = Vgs - Vt (nMOS)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -666,7 +672,7 @@
                   </a:sysClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Id en el punto Vds = Vgs - Vt</a:t>
+              <a:t>Id en el punto Vds = Vgs - Vt (nMOS)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1181,6 +1187,1045 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Id en el punto Vds = Vgs - Vt (pMOS)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.09</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.4000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-016E-411B-A78F-2718D8613D61}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1103392816"/>
+        <c:axId val="1103400496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1103392816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1103400496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1103400496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CL" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Ids (mA)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1103392816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Id en el punto Vds = Vgs - Vt (pMOS)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$2:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.09</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.4000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.316</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A730-4523-A48C-304595B43257}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1266599936"/>
+        <c:axId val="1266597056"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1266599936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CL" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Vds = Vgs - Vt (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1266597056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1266597056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CL" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Ids (mA)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1266599936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1261,6 +2306,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1778,6 +2903,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2362,6 +4519,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F24707FA-4CA5-1BAA-5F3A-225453EC1739}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85588548-3E4F-31E5-779C-F465B927429F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2687,15 +4916,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FA55D9-80E3-42C4-AC54-A07AEA5295F2}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="O2" sqref="O2:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2705,8 +4934,23 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.5</v>
       </c>
@@ -2716,8 +4960,18 @@
       <c r="C2">
         <v>0.16</v>
       </c>
+      <c r="N2">
+        <v>1.5</v>
+      </c>
+      <c r="O2">
+        <f>N2-0.91</f>
+        <v>0.59</v>
+      </c>
+      <c r="P2">
+        <v>3.4000000000000002E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2727,8 +4981,18 @@
       <c r="C3">
         <v>0.4</v>
       </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O9" si="0">N3-0.91</f>
+        <v>1.0899999999999999</v>
+      </c>
+      <c r="P3">
+        <v>0.10100000000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.5</v>
       </c>
@@ -2738,8 +5002,18 @@
       <c r="C4">
         <v>0.74</v>
       </c>
+      <c r="N4">
+        <v>2.5</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>1.5899999999999999</v>
+      </c>
+      <c r="P4">
+        <v>0.19600000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2749,8 +5023,18 @@
       <c r="C5">
         <v>1.1399999999999999</v>
       </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>2.09</v>
+      </c>
+      <c r="P5">
+        <v>0.316</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3.5</v>
       </c>
@@ -2760,8 +5044,18 @@
       <c r="C6">
         <v>1.6</v>
       </c>
+      <c r="N6">
+        <v>3.5</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>2.59</v>
+      </c>
+      <c r="P6">
+        <v>0.45800000000000002</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2771,8 +5065,18 @@
       <c r="C7">
         <v>2.08</v>
       </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>3.09</v>
+      </c>
+      <c r="P7">
+        <v>0.61699999999999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.5</v>
       </c>
@@ -2782,8 +5086,18 @@
       <c r="C8">
         <v>2.62</v>
       </c>
+      <c r="N8">
+        <v>4.5</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>3.59</v>
+      </c>
+      <c r="P8">
+        <v>0.79300000000000004</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2792,6 +5106,16 @@
       </c>
       <c r="C9">
         <v>3.19</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>4.09</v>
+      </c>
+      <c r="P9">
+        <v>0.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>